<commit_message>
got up to removing empty rows from analysisMetadata for new version
</commit_message>
<xml_diff>
--- a/raw-v3/FAIRe_NOAA_checklist_v1.0.xlsx
+++ b/raw-v3/FAIRe_NOAA_checklist_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4928F431-1613-49AD-8976-2C7D20BD25E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7264FBF6-D685-446A-A850-B90ADC635640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1155" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5264,7 +5264,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H313" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O327" sqref="O327"/>
+      <selection pane="bottomRight" activeCell="H358" sqref="H358"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
Works up to building of Occurrence table. empty rows deleted from analysis files too
</commit_message>
<xml_diff>
--- a/raw-v3/FAIRe_NOAA_checklist_v1.0.xlsx
+++ b/raw-v3/FAIRe_NOAA_checklist_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4928F431-1613-49AD-8976-2C7D20BD25E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7264FBF6-D685-446A-A850-B90ADC635640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1155" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5264,7 +5264,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H313" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O327" sqref="O327"/>
+      <selection pane="bottomRight" activeCell="H358" sqref="H358"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
DNA Derived Extension working completely
</commit_message>
<xml_diff>
--- a/raw-v3/FAIRe_NOAA_checklist_v1.0.xlsx
+++ b/raw-v3/FAIRe_NOAA_checklist_v1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6CB2CEF-AD7D-4193-BC98-A82F29163BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C526F0C-6D77-45B6-BE29-B1DDF6D28933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1155" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1475">
   <si>
     <t>Instructions for data submitters:</t>
   </si>
@@ -5269,8 +5269,8 @@
   <dimension ref="A1:R406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O40" sqref="O40"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I181" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="N189" sqref="N189"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -5287,7 +5287,7 @@
     <col min="8" max="8" width="36.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="37.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" customWidth="1"/>
+    <col min="11" max="11" width="118.5703125" customWidth="1"/>
     <col min="12" max="12" width="21.28515625" style="15" customWidth="1"/>
     <col min="13" max="13" width="29.85546875" style="15" customWidth="1"/>
     <col min="14" max="15" width="32.42578125" customWidth="1"/>
@@ -11884,6 +11884,9 @@
       <c r="L189" s="15" t="s">
         <v>772</v>
       </c>
+      <c r="N189" t="s">
+        <v>268</v>
+      </c>
       <c r="O189" t="s">
         <v>773</v>
       </c>

</xml_diff>